<commit_message>
opti: Add missing i18n
</commit_message>
<xml_diff>
--- a/src/data/i18n.xlsx
+++ b/src/data/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -86,6 +86,57 @@
   </si>
   <si>
     <t>About</t>
+  </si>
+  <si>
+    <t>navbar.feedback</t>
+  </si>
+  <si>
+    <t>反馈</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>channel.life</t>
+  </si>
+  <si>
+    <t>生活常用</t>
+  </si>
+  <si>
+    <t>Lifestyle</t>
+  </si>
+  <si>
+    <t>channel.ai</t>
+  </si>
+  <si>
+    <t>人工智能</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>channel.image</t>
+  </si>
+  <si>
+    <t>Media Process</t>
+  </si>
+  <si>
+    <t>channel.developer</t>
+  </si>
+  <si>
+    <t>编程开发</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>channel.external</t>
+  </si>
+  <si>
+    <t>第三方APP</t>
+  </si>
+  <si>
+    <t>External App</t>
   </si>
 </sst>
 </file>
@@ -155,7 +206,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -165,16 +216,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -394,17 +442,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -431,10 +479,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -673,12 +721,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -955,7 +1003,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -982,10 +1030,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1250,228 +1298,264 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="20.1" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="A2" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" ht="20.1" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" ht="20.1" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="A4" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" ht="20.1" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="A5" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" ht="20.1" customHeight="1">
-      <c r="A6" t="s" s="4">
+      <c r="A6" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="D6" t="s" s="4">
+      <c r="D6" t="s" s="3">
         <v>17</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" ht="20.1" customHeight="1">
-      <c r="A7" t="s" s="4">
+      <c r="A7" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" ht="20.1" customHeight="1">
-      <c r="A8" t="s" s="4">
+      <c r="A8" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" ht="20.1" customHeight="1">
-      <c r="A9" t="s" s="4">
+      <c r="A9" t="s" s="3">
         <v>22</v>
       </c>
-      <c r="B9" t="s" s="4">
+      <c r="B9" t="s" s="3">
         <v>23</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C9" t="s" s="3">
         <v>24</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" ht="20.1" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="A10" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" ht="20.1" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
+      <c r="A11" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" ht="20.1" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="A12" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" ht="20.1" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
+      <c r="A13" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" ht="20.1" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
+      <c r="A14" t="s" s="3">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" ht="20.1" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
+      <c r="A15" t="s" s="3">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s" s="3">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" ht="20.1" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" ht="20.1" customHeight="1">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" ht="20.1" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" ht="20.1" customHeight="1">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" ht="20.1" customHeight="1">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" ht="20.1" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" ht="20.1" customHeight="1">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" ht="20.1" customHeight="1">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" ht="20.1" customHeight="1">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" ht="20.1" customHeight="1">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" ht="20.1" customHeight="1">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Add language switch
</commit_message>
<xml_diff>
--- a/src/data/i18n.xlsx
+++ b/src/data/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +88,15 @@
     <t>About</t>
   </si>
   <si>
+    <t>navbar.settings</t>
+  </si>
+  <si>
+    <t>设置</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
     <t>navbar.feedback</t>
   </si>
   <si>
@@ -182,6 +191,36 @@
   </si>
   <si>
     <t>Remove Bookmark</t>
+  </si>
+  <si>
+    <t>settings.language.title</t>
+  </si>
+  <si>
+    <t>语言</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>settings.language.auto</t>
+  </si>
+  <si>
+    <t>跟随系统</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>settings.language.zh_cn</t>
+  </si>
+  <si>
+    <t>简体中文</t>
+  </si>
+  <si>
+    <t>settings.language.en_us</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
 </sst>
 </file>
@@ -1320,7 +1359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1504,20 +1543,20 @@
         <v>37</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" ht="20.1" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s" s="3">
         <v>41</v>
@@ -1591,37 +1630,67 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" ht="20.1" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s" s="3">
+        <v>59</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" ht="20.1" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s" s="3">
+        <v>62</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" ht="20.1" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" t="s" s="3">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s" s="3">
+        <v>65</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" ht="20.1" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A24" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s" s="3">
+        <v>67</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" ht="20.1" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="A25" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s" s="3">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s" s="3">
+        <v>69</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
     </row>
@@ -1645,6 +1714,13 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
+    </row>
+    <row r="29" ht="20.1" customHeight="1">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Send to email
</commit_message>
<xml_diff>
--- a/src/data/i18n.xlsx
+++ b/src/data/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -239,6 +239,51 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>feedback.send</t>
+  </si>
+  <si>
+    <t>提交</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>feedback.hero</t>
+  </si>
+  <si>
+    <t>我们会阅读每一条反馈</t>
+  </si>
+  <si>
+    <t>We Read Every Feedback</t>
+  </si>
+  <si>
+    <t>feedback.debug</t>
+  </si>
+  <si>
+    <t>发送错误日志</t>
+  </si>
+  <si>
+    <t>Send Error Log</t>
+  </si>
+  <si>
+    <t>feedback.content.placeholder</t>
+  </si>
+  <si>
+    <t>输入内容</t>
+  </si>
+  <si>
+    <t>Write something you want to tell us</t>
+  </si>
+  <si>
+    <t>feedback.contact.placeholder</t>
+  </si>
+  <si>
+    <t>适合我们联系你的方式</t>
+  </si>
+  <si>
+    <t>How can we contact you?</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1739,32 +1784,69 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" ht="20.1" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" t="s" s="3">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s" s="3">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s" s="3">
+        <v>78</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" ht="20.1" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="A29" t="s" s="3">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s" s="3">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s" s="3">
+        <v>81</v>
+      </c>
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" ht="20.1" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="A30" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s" s="3">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s" s="3">
+        <v>84</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" ht="20.1" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="A31" t="s" s="3">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s" s="3">
+        <v>87</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
+    </row>
+    <row r="32" ht="20.1" customHeight="1">
+      <c r="A32" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s" s="3">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s" s="3">
+        <v>90</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Switch locale for about page
</commit_message>
<xml_diff>
--- a/src/data/i18n.xlsx
+++ b/src/data/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -284,6 +284,120 @@
   </si>
   <si>
     <t>How can we contact you?</t>
+  </si>
+  <si>
+    <t>general.chooseFile</t>
+  </si>
+  <si>
+    <t>选择文件</t>
+  </si>
+  <si>
+    <t>Choose File</t>
+  </si>
+  <si>
+    <t>general.confirm</t>
+  </si>
+  <si>
+    <t>确认</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>general.save</t>
+  </si>
+  <si>
+    <t>保存</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>general.download</t>
+  </si>
+  <si>
+    <t>下载</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>qrcode.basic.title</t>
+  </si>
+  <si>
+    <t>基本</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>qrcode.basic.placeholder</t>
+  </si>
+  <si>
+    <t>链接或文本</t>
+  </si>
+  <si>
+    <t>URL or Text</t>
+  </si>
+  <si>
+    <t>qrcode.basic.type</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>qrcode.basic.wifi</t>
+  </si>
+  <si>
+    <t>WI-FI</t>
+  </si>
+  <si>
+    <t>qrcode.basic.text</t>
+  </si>
+  <si>
+    <t>文本</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>qrcode.advanced.title</t>
+  </si>
+  <si>
+    <t>高级</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>qrcode.advanced.icon</t>
+  </si>
+  <si>
+    <t>图标</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>qrcode.advanced.light</t>
+  </si>
+  <si>
+    <t>亮色</t>
+  </si>
+  <si>
+    <t>Light Color</t>
+  </si>
+  <si>
+    <t>qrcode.advanced.dark</t>
+  </si>
+  <si>
+    <t>暗色</t>
+  </si>
+  <si>
+    <t>Dark Color</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1848,6 +1962,175 @@
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
     </row>
+    <row r="33" ht="20.1" customHeight="1">
+      <c r="A33" t="s" s="3">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s" s="3">
+        <v>93</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" ht="20.1" customHeight="1">
+      <c r="A34" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s" s="3">
+        <v>95</v>
+      </c>
+      <c r="C34" t="s" s="3">
+        <v>96</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" ht="20.1" customHeight="1">
+      <c r="A35" t="s" s="3">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s" s="3">
+        <v>98</v>
+      </c>
+      <c r="C35" t="s" s="3">
+        <v>99</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" ht="20.1" customHeight="1">
+      <c r="A36" t="s" s="3">
+        <v>100</v>
+      </c>
+      <c r="B36" t="s" s="3">
+        <v>101</v>
+      </c>
+      <c r="C36" t="s" s="3">
+        <v>102</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" ht="20.1" customHeight="1">
+      <c r="A37" t="s" s="3">
+        <v>103</v>
+      </c>
+      <c r="B37" t="s" s="3">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s" s="3">
+        <v>105</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" ht="20.1" customHeight="1">
+      <c r="A38" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="B38" t="s" s="3">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s" s="3">
+        <v>108</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" ht="20.1" customHeight="1">
+      <c r="A39" t="s" s="3">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s" s="3">
+        <v>110</v>
+      </c>
+      <c r="C39" t="s" s="3">
+        <v>111</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" ht="20.1" customHeight="1">
+      <c r="A40" t="s" s="3">
+        <v>112</v>
+      </c>
+      <c r="B40" t="s" s="3">
+        <v>113</v>
+      </c>
+      <c r="C40" t="s" s="3">
+        <v>113</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" ht="20.1" customHeight="1">
+      <c r="A41" t="s" s="3">
+        <v>114</v>
+      </c>
+      <c r="B41" t="s" s="3">
+        <v>115</v>
+      </c>
+      <c r="C41" t="s" s="3">
+        <v>116</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" ht="20.1" customHeight="1">
+      <c r="A42" t="s" s="3">
+        <v>117</v>
+      </c>
+      <c r="B42" t="s" s="3">
+        <v>118</v>
+      </c>
+      <c r="C42" t="s" s="3">
+        <v>119</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" ht="20.1" customHeight="1">
+      <c r="A43" t="s" s="3">
+        <v>120</v>
+      </c>
+      <c r="B43" t="s" s="3">
+        <v>121</v>
+      </c>
+      <c r="C43" t="s" s="3">
+        <v>122</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" ht="20.1" customHeight="1">
+      <c r="A44" t="s" s="3">
+        <v>123</v>
+      </c>
+      <c r="B44" t="s" s="3">
+        <v>124</v>
+      </c>
+      <c r="C44" t="s" s="3">
+        <v>125</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" ht="20.1" customHeight="1">
+      <c r="A45" t="s" s="3">
+        <v>126</v>
+      </c>
+      <c r="B45" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s" s="3">
+        <v>128</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
feat: add missing strings
</commit_message>
<xml_diff>
--- a/src/data/i18n.xlsx
+++ b/src/data/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -37,7 +37,10 @@
     <t>homePage.meta.description</t>
   </si>
   <si>
-    <t>云极客工具，励志做最轻盈最好用的在线工具。以工匠精神打造功能丰富的在线工具，无需下载即可免费使用</t>
+    <t>轻盈好用的在线工具，无需下载即可免费使用，解决生活学习工作中的大小问题</t>
+  </si>
+  <si>
+    <t>Effortless solutions at your fingertips. Streamline your workflow with our intuitive online toolbox. No installation. No hassle. Just pure productivity.</t>
   </si>
   <si>
     <t>homePage.meta.title</t>
@@ -398,6 +401,9 @@
   </si>
   <si>
     <t>Dark Color</t>
+  </si>
+  <si>
+    <t>aboutPage.meta.title</t>
   </si>
 </sst>
 </file>
@@ -1536,7 +1542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1581,29 +1587,31 @@
       <c r="B3" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" t="s" s="3">
+        <v>9</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" ht="20.1" customHeight="1">
       <c r="A4" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" ht="20.1" customHeight="1">
       <c r="A5" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1611,525 +1619,538 @@
     </row>
     <row r="6" ht="20.1" customHeight="1">
       <c r="A6" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" ht="20.1" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" ht="20.1" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" ht="20.1" customHeight="1">
       <c r="A9" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" ht="20.1" customHeight="1">
       <c r="A10" t="s" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" ht="20.1" customHeight="1">
       <c r="A11" t="s" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" ht="20.1" customHeight="1">
       <c r="A12" t="s" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
     </row>
     <row r="13" ht="20.1" customHeight="1">
       <c r="A13" t="s" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" ht="20.1" customHeight="1">
       <c r="A14" t="s" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" ht="20.1" customHeight="1">
       <c r="A15" t="s" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" ht="20.1" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" ht="20.1" customHeight="1">
       <c r="A17" t="s" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s" s="3">
         <v>6</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" ht="20.1" customHeight="1">
       <c r="A18" t="s" s="3">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" ht="20.1" customHeight="1">
       <c r="A19" t="s" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" ht="20.1" customHeight="1">
       <c r="A20" t="s" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s" s="3">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" ht="20.1" customHeight="1">
       <c r="A21" t="s" s="3">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" ht="20.1" customHeight="1">
       <c r="A22" t="s" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s" s="3">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" ht="20.1" customHeight="1">
       <c r="A23" t="s" s="3">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s" s="3">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s" s="3">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" ht="20.1" customHeight="1">
       <c r="A24" t="s" s="3">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s" s="3">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" ht="20.1" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s" s="3">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s" s="3">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" ht="20.1" customHeight="1">
       <c r="A26" t="s" s="3">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s" s="3">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" ht="20.1" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s" s="3">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s" s="3">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" ht="20.1" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s" s="3">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" ht="20.1" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s" s="3">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" ht="20.1" customHeight="1">
       <c r="A30" t="s" s="3">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s" s="3">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" ht="20.1" customHeight="1">
       <c r="A31" t="s" s="3">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s" s="3">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s" s="3">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" ht="20.1" customHeight="1">
       <c r="A32" t="s" s="3">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s" s="3">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s" s="3">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" ht="20.1" customHeight="1">
       <c r="A33" t="s" s="3">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s" s="3">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s" s="3">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" ht="20.1" customHeight="1">
       <c r="A34" t="s" s="3">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s" s="3">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s" s="3">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" ht="20.1" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s" s="3">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s" s="3">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" ht="20.1" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s" s="3">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s" s="3">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" ht="20.1" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s" s="3">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s" s="3">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" ht="20.1" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s" s="3">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s" s="3">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" ht="20.1" customHeight="1">
       <c r="A39" t="s" s="3">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s" s="3">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s" s="3">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" ht="20.1" customHeight="1">
       <c r="A40" t="s" s="3">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s" s="3">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s" s="3">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" ht="20.1" customHeight="1">
       <c r="A41" t="s" s="3">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B41" t="s" s="3">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s" s="3">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" ht="20.1" customHeight="1">
       <c r="A42" t="s" s="3">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s" s="3">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s" s="3">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" ht="20.1" customHeight="1">
       <c r="A43" t="s" s="3">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s" s="3">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s" s="3">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" ht="20.1" customHeight="1">
       <c r="A44" t="s" s="3">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s" s="3">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C44" t="s" s="3">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" ht="20.1" customHeight="1">
       <c r="A45" t="s" s="3">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s" s="3">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C45" t="s" s="3">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="5"/>
+    </row>
+    <row r="46" ht="20.1" customHeight="1">
+      <c r="A46" t="s" s="3">
+        <v>130</v>
+      </c>
+      <c r="B46" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="C46" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: app download CTA
</commit_message>
<xml_diff>
--- a/src/data/i18n.xlsx
+++ b/src/data/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -104,6 +104,24 @@
   </si>
   <si>
     <t>Settings</t>
+  </si>
+  <si>
+    <t>navbar.downloadApp.tooltip</t>
+  </si>
+  <si>
+    <t>Geekits APP 带来更快的速度，离线使用，以及更好的体验</t>
+  </si>
+  <si>
+    <t>Geekits app allows faster access, offline use, and more.</t>
+  </si>
+  <si>
+    <t>navbar.downloadApp.label</t>
+  </si>
+  <si>
+    <t>试试 Geekits APP</t>
+  </si>
+  <si>
+    <t>Try Geekits App</t>
   </si>
   <si>
     <t>navbar.feedback</t>
@@ -551,7 +569,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -575,6 +593,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1626,14 +1650,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="40.6719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.8984" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.8516" style="1" customWidth="1"/>
     <col min="3" max="5" width="40.6719" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
@@ -1781,18 +1805,18 @@
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" ht="20.1" customHeight="1">
-      <c r="A12" t="s" s="4">
+    <row r="12" ht="35" customHeight="1">
+      <c r="A12" t="s" s="5">
         <v>31</v>
       </c>
       <c r="B12" t="s" s="5">
         <v>32</v>
       </c>
-      <c r="C12" t="s" s="4">
+      <c r="C12" t="s" s="5">
         <v>33</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" ht="20.1" customHeight="1">
       <c r="A13" t="s" s="4">
@@ -1864,33 +1888,33 @@
         <v>49</v>
       </c>
       <c r="B18" t="s" s="5">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
     </row>
     <row r="19" ht="20.1" customHeight="1">
       <c r="A19" t="s" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s" s="5">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s" s="4">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
     </row>
     <row r="20" ht="20.1" customHeight="1">
       <c r="A20" t="s" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s" s="5">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s" s="4">
         <v>56</v>
@@ -1984,43 +2008,43 @@
         <v>76</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28" ht="20.1" customHeight="1">
       <c r="A28" t="s" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s" s="5">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
     </row>
     <row r="29" ht="20.1" customHeight="1">
       <c r="A29" t="s" s="4">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s" s="5">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
     </row>
     <row r="30" ht="20.1" customHeight="1">
       <c r="A30" t="s" s="4">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s" s="5">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s" s="4">
         <v>84</v>
@@ -2192,30 +2216,30 @@
         <v>122</v>
       </c>
       <c r="C43" t="s" s="4">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="7"/>
     </row>
     <row r="44" ht="20.1" customHeight="1">
       <c r="A44" t="s" s="4">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s" s="5">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C44" t="s" s="4">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="7"/>
     </row>
     <row r="45" ht="20.1" customHeight="1">
       <c r="A45" t="s" s="4">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s" s="5">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C45" t="s" s="4">
         <v>128</v>
@@ -2267,36 +2291,36 @@
         <v>138</v>
       </c>
       <c r="B49" t="s" s="5">
-        <v>26</v>
+        <v>139</v>
       </c>
       <c r="C49" t="s" s="4">
-        <v>27</v>
+        <v>140</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="7"/>
     </row>
     <row r="50" ht="20.1" customHeight="1">
       <c r="A50" t="s" s="4">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s" s="5">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s" s="4">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51" ht="20.1" customHeight="1">
       <c r="A51" t="s" s="4">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s" s="5">
-        <v>143</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s" s="4">
-        <v>144</v>
+        <v>27</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="7"/>
@@ -2352,6 +2376,32 @@
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="7"/>
+    </row>
+    <row r="56" ht="20.1" customHeight="1">
+      <c r="A56" t="s" s="4">
+        <v>157</v>
+      </c>
+      <c r="B56" t="s" s="5">
+        <v>158</v>
+      </c>
+      <c r="C56" t="s" s="4">
+        <v>159</v>
+      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" ht="20.1" customHeight="1">
+      <c r="A57" t="s" s="4">
+        <v>160</v>
+      </c>
+      <c r="B57" t="s" s="5">
+        <v>161</v>
+      </c>
+      <c r="C57" t="s" s="4">
+        <v>162</v>
+      </c>
+      <c r="D57" s="6"/>
+      <c r="E57" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Add external app
</commit_message>
<xml_diff>
--- a/src/data/i18n.xlsx
+++ b/src/data/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="185">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,15 @@
     <t>What’s New</t>
   </si>
   <si>
+    <t>navbar.more.title</t>
+  </si>
+  <si>
+    <t>更多 YGeeker 产品</t>
+  </si>
+  <si>
+    <t>More Products from YGeeker</t>
+  </si>
+  <si>
     <t>channel.life</t>
   </si>
   <si>
@@ -196,7 +205,7 @@
     <t>channel.external</t>
   </si>
   <si>
-    <t>第三方APP</t>
+    <t>外部 APP</t>
   </si>
   <si>
     <t>External App</t>
@@ -539,6 +548,24 @@
   </si>
   <si>
     <t>Color Revert</t>
+  </si>
+  <si>
+    <t>app.hotpot.addDish</t>
+  </si>
+  <si>
+    <t>从预设菜品中选择</t>
+  </si>
+  <si>
+    <t>Add Preset Dish</t>
+  </si>
+  <si>
+    <t>account.dialog.title</t>
+  </si>
+  <si>
+    <t>YGeeker 账户</t>
+  </si>
+  <si>
+    <t>YGeeker Account</t>
   </si>
 </sst>
 </file>
@@ -1689,7 +1716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1953,20 +1980,20 @@
         <v>55</v>
       </c>
       <c r="B20" t="s" s="5">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" ht="20.1" customHeight="1">
       <c r="A21" t="s" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s" s="5">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s" s="4">
         <v>59</v>
@@ -2044,23 +2071,23 @@
         <v>75</v>
       </c>
       <c r="B27" t="s" s="5">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28" ht="20.1" customHeight="1">
       <c r="A28" t="s" s="4">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s" s="5">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
@@ -2099,30 +2126,30 @@
         <v>86</v>
       </c>
       <c r="C31" t="s" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
     </row>
     <row r="32" ht="20.1" customHeight="1">
       <c r="A32" t="s" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s" s="5">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
     </row>
     <row r="33" ht="20.1" customHeight="1">
       <c r="A33" t="s" s="4">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s" s="5">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s" s="4">
         <v>91</v>
@@ -2307,17 +2334,17 @@
         <v>132</v>
       </c>
       <c r="C47" t="s" s="4">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7"/>
     </row>
     <row r="48" ht="20.1" customHeight="1">
       <c r="A48" t="s" s="4">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s" s="5">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C48" t="s" s="4">
         <v>135</v>
@@ -2382,23 +2409,23 @@
         <v>148</v>
       </c>
       <c r="B53" t="s" s="5">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="C53" t="s" s="4">
-        <v>27</v>
+        <v>150</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" ht="20.1" customHeight="1">
       <c r="A54" t="s" s="4">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B54" t="s" s="5">
-        <v>150</v>
+        <v>26</v>
       </c>
       <c r="C54" t="s" s="4">
-        <v>151</v>
+        <v>27</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="7"/>
@@ -2506,6 +2533,45 @@
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="7"/>
+    </row>
+    <row r="63" ht="20.1" customHeight="1">
+      <c r="A63" t="s" s="4">
+        <v>176</v>
+      </c>
+      <c r="B63" t="s" s="5">
+        <v>177</v>
+      </c>
+      <c r="C63" t="s" s="4">
+        <v>178</v>
+      </c>
+      <c r="D63" s="6"/>
+      <c r="E63" s="7"/>
+    </row>
+    <row r="64" ht="20.1" customHeight="1">
+      <c r="A64" t="s" s="4">
+        <v>179</v>
+      </c>
+      <c r="B64" t="s" s="5">
+        <v>180</v>
+      </c>
+      <c r="C64" t="s" s="4">
+        <v>181</v>
+      </c>
+      <c r="D64" s="6"/>
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" ht="20.1" customHeight="1">
+      <c r="A65" t="s" s="4">
+        <v>182</v>
+      </c>
+      <c r="B65" t="s" s="5">
+        <v>183</v>
+      </c>
+      <c r="C65" t="s" s="4">
+        <v>184</v>
+      </c>
+      <c r="D65" s="6"/>
+      <c r="E65" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
style: Update global visual styles
</commit_message>
<xml_diff>
--- a/src/data/i18n.xlsx
+++ b/src/data/i18n.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="195">
   <si>
     <t>Name</t>
   </si>
@@ -287,6 +287,36 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>settings.theme.title</t>
+  </si>
+  <si>
+    <t>主题</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>settings.theme.system</t>
+  </si>
+  <si>
+    <t>settings.theme.light</t>
+  </si>
+  <si>
+    <t>浅色</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>settings.theme.dark</t>
+  </si>
+  <si>
+    <t>深色</t>
+  </si>
+  <si>
+    <t>Dark</t>
   </si>
   <si>
     <t>donation.paid.title</t>
@@ -1716,7 +1746,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2175,257 +2205,257 @@
         <v>95</v>
       </c>
       <c r="B35" t="s" s="5">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s" s="4">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="7"/>
     </row>
     <row r="36" ht="20.1" customHeight="1">
       <c r="A36" t="s" s="4">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s" s="5">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s" s="4">
         <v>98</v>
-      </c>
-      <c r="B36" t="s" s="5">
-        <v>99</v>
-      </c>
-      <c r="C36" t="s" s="4">
-        <v>100</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="7"/>
     </row>
     <row r="37" ht="20.1" customHeight="1">
       <c r="A37" t="s" s="4">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s" s="5">
+        <v>100</v>
+      </c>
+      <c r="C37" t="s" s="4">
         <v>101</v>
-      </c>
-      <c r="B37" t="s" s="5">
-        <v>102</v>
-      </c>
-      <c r="C37" t="s" s="4">
-        <v>103</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="7"/>
     </row>
     <row r="38" ht="20.1" customHeight="1">
       <c r="A38" t="s" s="4">
+        <v>102</v>
+      </c>
+      <c r="B38" t="s" s="5">
+        <v>103</v>
+      </c>
+      <c r="C38" t="s" s="4">
         <v>104</v>
-      </c>
-      <c r="B38" t="s" s="5">
-        <v>105</v>
-      </c>
-      <c r="C38" t="s" s="4">
-        <v>106</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39" ht="20.1" customHeight="1">
       <c r="A39" t="s" s="4">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s" s="5">
+        <v>106</v>
+      </c>
+      <c r="C39" t="s" s="4">
         <v>107</v>
-      </c>
-      <c r="B39" t="s" s="5">
-        <v>108</v>
-      </c>
-      <c r="C39" t="s" s="4">
-        <v>109</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
     </row>
     <row r="40" ht="20.1" customHeight="1">
       <c r="A40" t="s" s="4">
+        <v>108</v>
+      </c>
+      <c r="B40" t="s" s="5">
+        <v>109</v>
+      </c>
+      <c r="C40" t="s" s="4">
         <v>110</v>
-      </c>
-      <c r="B40" t="s" s="5">
-        <v>111</v>
-      </c>
-      <c r="C40" t="s" s="4">
-        <v>112</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" ht="20.1" customHeight="1">
       <c r="A41" t="s" s="4">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s" s="5">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s" s="4">
         <v>113</v>
-      </c>
-      <c r="B41" t="s" s="5">
-        <v>114</v>
-      </c>
-      <c r="C41" t="s" s="4">
-        <v>115</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
     </row>
     <row r="42" ht="20.1" customHeight="1">
       <c r="A42" t="s" s="4">
+        <v>114</v>
+      </c>
+      <c r="B42" t="s" s="5">
+        <v>115</v>
+      </c>
+      <c r="C42" t="s" s="4">
         <v>116</v>
-      </c>
-      <c r="B42" t="s" s="5">
-        <v>117</v>
-      </c>
-      <c r="C42" t="s" s="4">
-        <v>118</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="7"/>
     </row>
     <row r="43" ht="20.1" customHeight="1">
       <c r="A43" t="s" s="4">
+        <v>117</v>
+      </c>
+      <c r="B43" t="s" s="5">
+        <v>118</v>
+      </c>
+      <c r="C43" t="s" s="4">
         <v>119</v>
-      </c>
-      <c r="B43" t="s" s="5">
-        <v>120</v>
-      </c>
-      <c r="C43" t="s" s="4">
-        <v>121</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="7"/>
     </row>
     <row r="44" ht="20.1" customHeight="1">
       <c r="A44" t="s" s="4">
+        <v>120</v>
+      </c>
+      <c r="B44" t="s" s="5">
+        <v>121</v>
+      </c>
+      <c r="C44" t="s" s="4">
         <v>122</v>
-      </c>
-      <c r="B44" t="s" s="5">
-        <v>123</v>
-      </c>
-      <c r="C44" t="s" s="4">
-        <v>124</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="7"/>
     </row>
     <row r="45" ht="20.1" customHeight="1">
       <c r="A45" t="s" s="4">
+        <v>123</v>
+      </c>
+      <c r="B45" t="s" s="5">
+        <v>124</v>
+      </c>
+      <c r="C45" t="s" s="4">
         <v>125</v>
-      </c>
-      <c r="B45" t="s" s="5">
-        <v>126</v>
-      </c>
-      <c r="C45" t="s" s="4">
-        <v>127</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
     </row>
     <row r="46" ht="20.1" customHeight="1">
       <c r="A46" t="s" s="4">
+        <v>126</v>
+      </c>
+      <c r="B46" t="s" s="5">
+        <v>127</v>
+      </c>
+      <c r="C46" t="s" s="4">
         <v>128</v>
-      </c>
-      <c r="B46" t="s" s="5">
-        <v>129</v>
-      </c>
-      <c r="C46" t="s" s="4">
-        <v>130</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
     </row>
     <row r="47" ht="20.1" customHeight="1">
       <c r="A47" t="s" s="4">
+        <v>129</v>
+      </c>
+      <c r="B47" t="s" s="5">
+        <v>130</v>
+      </c>
+      <c r="C47" t="s" s="4">
         <v>131</v>
-      </c>
-      <c r="B47" t="s" s="5">
-        <v>132</v>
-      </c>
-      <c r="C47" t="s" s="4">
-        <v>133</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="7"/>
     </row>
     <row r="48" ht="20.1" customHeight="1">
       <c r="A48" t="s" s="4">
+        <v>132</v>
+      </c>
+      <c r="B48" t="s" s="5">
+        <v>133</v>
+      </c>
+      <c r="C48" t="s" s="4">
         <v>134</v>
-      </c>
-      <c r="B48" t="s" s="5">
-        <v>135</v>
-      </c>
-      <c r="C48" t="s" s="4">
-        <v>135</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
     </row>
     <row r="49" ht="20.1" customHeight="1">
       <c r="A49" t="s" s="4">
+        <v>135</v>
+      </c>
+      <c r="B49" t="s" s="5">
         <v>136</v>
       </c>
-      <c r="B49" t="s" s="5">
+      <c r="C49" t="s" s="4">
         <v>137</v>
-      </c>
-      <c r="C49" t="s" s="4">
-        <v>138</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="7"/>
     </row>
     <row r="50" ht="20.1" customHeight="1">
       <c r="A50" t="s" s="4">
+        <v>138</v>
+      </c>
+      <c r="B50" t="s" s="5">
         <v>139</v>
       </c>
-      <c r="B50" t="s" s="5">
+      <c r="C50" t="s" s="4">
         <v>140</v>
-      </c>
-      <c r="C50" t="s" s="4">
-        <v>141</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51" ht="20.1" customHeight="1">
       <c r="A51" t="s" s="4">
+        <v>141</v>
+      </c>
+      <c r="B51" t="s" s="5">
         <v>142</v>
       </c>
-      <c r="B51" t="s" s="5">
+      <c r="C51" t="s" s="4">
         <v>143</v>
-      </c>
-      <c r="C51" t="s" s="4">
-        <v>144</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="7"/>
     </row>
     <row r="52" ht="20.1" customHeight="1">
       <c r="A52" t="s" s="4">
+        <v>144</v>
+      </c>
+      <c r="B52" t="s" s="5">
         <v>145</v>
       </c>
-      <c r="B52" t="s" s="5">
-        <v>146</v>
-      </c>
       <c r="C52" t="s" s="4">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="7"/>
     </row>
     <row r="53" ht="20.1" customHeight="1">
       <c r="A53" t="s" s="4">
+        <v>146</v>
+      </c>
+      <c r="B53" t="s" s="5">
+        <v>147</v>
+      </c>
+      <c r="C53" t="s" s="4">
         <v>148</v>
-      </c>
-      <c r="B53" t="s" s="5">
-        <v>149</v>
-      </c>
-      <c r="C53" t="s" s="4">
-        <v>150</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" ht="20.1" customHeight="1">
       <c r="A54" t="s" s="4">
+        <v>149</v>
+      </c>
+      <c r="B54" t="s" s="5">
+        <v>150</v>
+      </c>
+      <c r="C54" t="s" s="4">
         <v>151</v>
-      </c>
-      <c r="B54" t="s" s="5">
-        <v>26</v>
-      </c>
-      <c r="C54" t="s" s="4">
-        <v>27</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="7"/>
@@ -2474,104 +2504,156 @@
         <v>161</v>
       </c>
       <c r="B58" t="s" s="5">
-        <v>162</v>
+        <v>26</v>
       </c>
       <c r="C58" t="s" s="4">
-        <v>163</v>
+        <v>27</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="7"/>
     </row>
     <row r="59" ht="20.1" customHeight="1">
       <c r="A59" t="s" s="4">
+        <v>162</v>
+      </c>
+      <c r="B59" t="s" s="5">
+        <v>163</v>
+      </c>
+      <c r="C59" t="s" s="4">
         <v>164</v>
-      </c>
-      <c r="B59" t="s" s="5">
-        <v>165</v>
-      </c>
-      <c r="C59" t="s" s="4">
-        <v>166</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="7"/>
     </row>
     <row r="60" ht="20.1" customHeight="1">
       <c r="A60" t="s" s="4">
+        <v>165</v>
+      </c>
+      <c r="B60" t="s" s="5">
+        <v>166</v>
+      </c>
+      <c r="C60" t="s" s="4">
         <v>167</v>
-      </c>
-      <c r="B60" t="s" s="5">
-        <v>168</v>
-      </c>
-      <c r="C60" t="s" s="4">
-        <v>169</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="7"/>
     </row>
     <row r="61" ht="20.1" customHeight="1">
       <c r="A61" t="s" s="4">
+        <v>168</v>
+      </c>
+      <c r="B61" t="s" s="5">
+        <v>169</v>
+      </c>
+      <c r="C61" t="s" s="4">
         <v>170</v>
-      </c>
-      <c r="B61" t="s" s="5">
-        <v>171</v>
-      </c>
-      <c r="C61" t="s" s="4">
-        <v>172</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="7"/>
     </row>
     <row r="62" ht="20.1" customHeight="1">
       <c r="A62" t="s" s="4">
+        <v>171</v>
+      </c>
+      <c r="B62" t="s" s="5">
+        <v>172</v>
+      </c>
+      <c r="C62" t="s" s="4">
         <v>173</v>
-      </c>
-      <c r="B62" t="s" s="5">
-        <v>174</v>
-      </c>
-      <c r="C62" t="s" s="4">
-        <v>175</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="7"/>
     </row>
     <row r="63" ht="20.1" customHeight="1">
       <c r="A63" t="s" s="4">
+        <v>174</v>
+      </c>
+      <c r="B63" t="s" s="5">
+        <v>175</v>
+      </c>
+      <c r="C63" t="s" s="4">
         <v>176</v>
-      </c>
-      <c r="B63" t="s" s="5">
-        <v>177</v>
-      </c>
-      <c r="C63" t="s" s="4">
-        <v>178</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="7"/>
     </row>
     <row r="64" ht="20.1" customHeight="1">
       <c r="A64" t="s" s="4">
+        <v>177</v>
+      </c>
+      <c r="B64" t="s" s="5">
+        <v>178</v>
+      </c>
+      <c r="C64" t="s" s="4">
         <v>179</v>
-      </c>
-      <c r="B64" t="s" s="5">
-        <v>180</v>
-      </c>
-      <c r="C64" t="s" s="4">
-        <v>181</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="7"/>
     </row>
     <row r="65" ht="20.1" customHeight="1">
       <c r="A65" t="s" s="4">
+        <v>180</v>
+      </c>
+      <c r="B65" t="s" s="5">
+        <v>181</v>
+      </c>
+      <c r="C65" t="s" s="4">
         <v>182</v>
-      </c>
-      <c r="B65" t="s" s="5">
-        <v>183</v>
-      </c>
-      <c r="C65" t="s" s="4">
-        <v>184</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="7"/>
+    </row>
+    <row r="66" ht="20.1" customHeight="1">
+      <c r="A66" t="s" s="4">
+        <v>183</v>
+      </c>
+      <c r="B66" t="s" s="5">
+        <v>184</v>
+      </c>
+      <c r="C66" t="s" s="4">
+        <v>185</v>
+      </c>
+      <c r="D66" s="6"/>
+      <c r="E66" s="7"/>
+    </row>
+    <row r="67" ht="20.1" customHeight="1">
+      <c r="A67" t="s" s="4">
+        <v>186</v>
+      </c>
+      <c r="B67" t="s" s="5">
+        <v>187</v>
+      </c>
+      <c r="C67" t="s" s="4">
+        <v>188</v>
+      </c>
+      <c r="D67" s="6"/>
+      <c r="E67" s="7"/>
+    </row>
+    <row r="68" ht="20.1" customHeight="1">
+      <c r="A68" t="s" s="4">
+        <v>189</v>
+      </c>
+      <c r="B68" t="s" s="5">
+        <v>190</v>
+      </c>
+      <c r="C68" t="s" s="4">
+        <v>191</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68" s="7"/>
+    </row>
+    <row r="69" ht="20.1" customHeight="1">
+      <c r="A69" t="s" s="4">
+        <v>192</v>
+      </c>
+      <c r="B69" t="s" s="5">
+        <v>193</v>
+      </c>
+      <c r="C69" t="s" s="4">
+        <v>194</v>
+      </c>
+      <c r="D69" s="6"/>
+      <c r="E69" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>